<commit_message>
M3 Cord Production System #527 - M3.Cord.Production.App re-implements #320
</commit_message>
<xml_diff>
--- a/Documents/Cord/Cord Imports/S1ConditionStd.xlsx
+++ b/Documents/Cord/Cord Imports/S1ConditionStd.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="39">
   <si>
     <t>ProcessName</t>
   </si>
@@ -115,6 +115,37 @@
   </si>
   <si>
     <t>StdValue</t>
+  </si>
+  <si>
+    <t>LifterChangeGearA</t>
+  </si>
+  <si>
+    <t>LifterChangeGearB</t>
+  </si>
+  <si>
+    <t>OuterDiameter</t>
+  </si>
+  <si>
+    <t>TravellerNo</t>
+  </si>
+  <si>
+    <t>RK - 500 J x 1 Pcs.</t>
+  </si>
+  <si>
+    <t>CouterUnit</t>
+  </si>
+  <si>
+    <t>CouterWeight</t>
+  </si>
+  <si>
+    <t>NumberRange</t>
+  </si>
+  <si>
+    <t>CounterSystem</t>
+  </si>
+  <si>
+    <t>เมื่อด้ายเต็ม Counter ที่ตั้งไว้
+เครื่องต้องหยุดและมีสัญญาณไฟเตือน</t>
   </si>
 </sst>
 </file>
@@ -165,9 +196,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
@@ -462,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -580,6 +615,152 @@
       </c>
       <c r="F5">
         <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>20120</v>
+      </c>
+      <c r="G10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>4.5</v>
+      </c>
+      <c r="G11">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="72">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>